<commit_message>
Finalized all Code Scripts
Download all code files, and run the main.py script to begin training
</commit_message>
<xml_diff>
--- a/Testing_Result.xlsx
+++ b/Testing_Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomng\Desktop\ChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472D3E7-99CA-40C9-A615-D1C142197658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7942D2-6DF0-42F6-A8B3-3BD43D1DF507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -332,44 +332,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>10760.802361173681</v>
-      </c>
-      <c r="B1">
-        <v>1481.252135103543</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10439.516188059109</v>
-      </c>
-      <c r="B2">
-        <v>1583.731394621698</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10087.3888299872</v>
-      </c>
-      <c r="B3">
-        <v>1482.266073047133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1763.142744541236</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>